<commit_message>
features completed except analysis
</commit_message>
<xml_diff>
--- a/DATA_BUKU.xlsx
+++ b/DATA_BUKU.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -391,13 +391,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G419"/>
+  <dimension ref="A1:G426"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D421" sqref="D421"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="3.77734375"/>
     <col customWidth="1" max="2" min="2" width="47.44140625"/>
@@ -435,7 +435,7 @@
       </c>
       <c r="F1" s="3" t="inlineStr">
         <is>
-          <t>Tick</t>
+          <t>/</t>
         </is>
       </c>
       <c r="G1" s="3" t="inlineStr">
@@ -461,6 +461,11 @@
       <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -479,6 +484,11 @@
       <c r="D3" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -520,6 +530,11 @@
       <c r="D5" s="2" t="n">
         <v>18</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -538,6 +553,11 @@
       <c r="D6" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -556,6 +576,11 @@
       <c r="D7" s="2" t="n">
         <v>10</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -574,6 +599,11 @@
       <c r="D8" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -592,6 +622,11 @@
       <c r="D9" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1240,9 +1275,6 @@
       <c r="D45" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="E45" s="3" t="inlineStr"/>
-      <c r="F45" s="3" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -1261,9 +1293,6 @@
       <c r="D46" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E46" s="3" t="inlineStr"/>
-      <c r="F46" s="3" t="inlineStr"/>
-      <c r="G46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -1302,9 +1331,6 @@
       <c r="D48" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E48" s="3" t="inlineStr"/>
-      <c r="F48" s="3" t="inlineStr"/>
-      <c r="G48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -1325,9 +1351,6 @@
           <t>FREE</t>
         </is>
       </c>
-      <c r="E49" s="3" t="inlineStr"/>
-      <c r="F49" s="3" t="inlineStr"/>
-      <c r="G49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -1346,9 +1369,6 @@
       <c r="D50" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E50" s="3" t="inlineStr"/>
-      <c r="F50" s="3" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -8099,6 +8119,13 @@
         <v>4</v>
       </c>
     </row>
+    <row r="420"/>
+    <row r="421"/>
+    <row r="422"/>
+    <row r="423"/>
+    <row r="424"/>
+    <row r="425"/>
+    <row r="426"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
bug with longer char coord  is fixed temporarily.
</commit_message>
<xml_diff>
--- a/DATA_BUKU.xlsx
+++ b/DATA_BUKU.xlsx
@@ -391,7 +391,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G426"/>
+  <dimension ref="A1:G419"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D421" sqref="D421"/>
@@ -699,6 +699,11 @@
       <c r="D13" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -8119,13 +8124,6 @@
         <v>4</v>
       </c>
     </row>
-    <row r="420"/>
-    <row r="421"/>
-    <row r="422"/>
-    <row r="423"/>
-    <row r="424"/>
-    <row r="425"/>
-    <row r="426"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Feature fixed, feat 3 still bugged, feat 4 not implemented yet
</commit_message>
<xml_diff>
--- a/DATA_BUKU.xlsx
+++ b/DATA_BUKU.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="181029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -391,10 +391,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G419"/>
+  <dimension ref="A1:G422"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D421" sqref="D421"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
@@ -433,11 +433,6 @@
           <t>Harga Jualan</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
       <c r="G1" s="3" t="inlineStr">
         <is>
           <t>Pembeli</t>
@@ -902,6 +897,11 @@
       <c r="D24" s="2" t="n">
         <v>8</v>
       </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -2168,6 +2168,11 @@
       <c r="D92" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="n">
@@ -4070,6 +4075,11 @@
       <c r="D195" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="1" t="n">
@@ -4244,6 +4254,11 @@
       <c r="D204" s="2" t="n">
         <v>5</v>
       </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
@@ -4340,6 +4355,11 @@
       <c r="D209" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
@@ -4772,6 +4792,11 @@
       <c r="D233" s="2" t="n">
         <v>3</v>
       </c>
+      <c r="F233" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
@@ -4790,6 +4815,11 @@
       <c r="D234" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F234" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
@@ -5122,6 +5152,11 @@
       <c r="D252" s="2" t="n">
         <v>2</v>
       </c>
+      <c r="F252" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
@@ -5358,6 +5393,11 @@
       <c r="D265" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F265" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
@@ -5736,6 +5776,11 @@
       <c r="D286" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
@@ -5754,6 +5799,11 @@
       <c r="D287" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
@@ -7237,6 +7287,11 @@
       <c r="D370" s="2" t="n">
         <v>4</v>
       </c>
+      <c r="F370" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
@@ -8124,6 +8179,21 @@
         <v>4</v>
       </c>
     </row>
+    <row r="420">
+      <c r="F420" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="F421" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+    </row>
+    <row r="422"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>

</xml_diff>